<commit_message>
Uvoz IGK za Puma
</commit_message>
<xml_diff>
--- a/Data-Puma/IDT_puma.xlsx
+++ b/Data-Puma/IDT_puma.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Exchange rate: EUR/USD</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Investing cash flows</t>
   </si>
   <si>
-    <t xml:space="preserve"> ∟ Increase/Decrease Other Long Term Assets</t>
-  </si>
-  <si>
     <t>Financing cash flows</t>
   </si>
   <si>
@@ -59,15 +56,9 @@
     <t>Funds from Operations before WC Changes &amp; Extra.</t>
   </si>
   <si>
-    <t>Dec/Inc in Receivables</t>
-  </si>
-  <si>
     <t>Dec/Inc in Inventories</t>
   </si>
   <si>
-    <t>Inc/Dec in Accounts Payable</t>
-  </si>
-  <si>
     <t>Inc/Dec in Other Accruals</t>
   </si>
   <si>
@@ -111,6 +102,9 @@
   </si>
   <si>
     <t>Cash &amp; Equivalents at End of Year</t>
+  </si>
+  <si>
+    <t>Increase/Decrease Other Long Term Assets</t>
   </si>
 </sst>
 </file>
@@ -135,11 +129,15 @@
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF555555"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="3">
@@ -483,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,7 +543,7 @@
     </row>
     <row r="4" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="6">
         <v>469131.778907776</v>
@@ -565,7 +563,7 @@
     </row>
     <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="6">
         <v>276805.72395324701</v>
@@ -585,7 +583,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="6">
         <v>45947.054016590097</v>
@@ -605,7 +603,7 @@
     </row>
     <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="6">
         <v>791884.55687761295</v>
@@ -625,411 +623,371 @@
     </row>
     <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="B8" s="6">
+        <v>-212097.892379761</v>
+      </c>
+      <c r="C8" s="6">
+        <v>-140606.07085228001</v>
+      </c>
+      <c r="D8" s="6">
+        <v>-140557.910060883</v>
+      </c>
+      <c r="E8" s="6">
+        <v>-60821.544599533103</v>
       </c>
       <c r="F8" s="6">
-        <v>-9580.5594444274902</v>
+        <v>-100378.134179115</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="6">
-        <v>-212097.892379761</v>
+        <v>240519.908678532</v>
       </c>
       <c r="C9" s="6">
-        <v>-140606.07085228001</v>
+        <v>167170.08423805199</v>
       </c>
       <c r="D9" s="6">
-        <v>-140557.910060883</v>
+        <v>191168.35207939101</v>
       </c>
       <c r="E9" s="6">
-        <v>-60821.544599533103</v>
-      </c>
-      <c r="F9" s="6">
-        <v>-100378.134179115</v>
+        <v>78214.187335968003</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="6">
+        <v>-203784.733462334</v>
+      </c>
+      <c r="C10" s="6">
+        <v>-163964.08262252799</v>
+      </c>
+      <c r="D10" s="6">
+        <v>-175097.73778915399</v>
+      </c>
+      <c r="E10" s="6">
+        <v>-67040.732002258301</v>
+      </c>
+      <c r="F10" s="6">
+        <v>-38757.717752456701</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="6">
-        <v>-26237.6684784889</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="B11" s="6">
+        <v>616521.83971404994</v>
+      </c>
+      <c r="C11" s="6">
+        <v>318424.66045618098</v>
+      </c>
+      <c r="D11" s="6">
+        <v>272480.86318969697</v>
+      </c>
+      <c r="E11" s="6">
+        <v>138087.04233169599</v>
+      </c>
+      <c r="F11" s="6">
+        <v>-40390.767657756798</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="6">
-        <v>240519.908678532</v>
-      </c>
-      <c r="C11" s="6">
-        <v>167170.08423805199</v>
-      </c>
-      <c r="D11" s="6">
-        <v>191168.35207939101</v>
-      </c>
-      <c r="E11" s="6">
-        <v>78214.187335968003</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="6">
-        <v>-203784.733462334</v>
-      </c>
-      <c r="C12" s="6">
-        <v>-163964.08262252799</v>
-      </c>
-      <c r="D12" s="6">
-        <v>-175097.73778915399</v>
-      </c>
-      <c r="E12" s="6">
-        <v>-67040.732002258301</v>
-      </c>
-      <c r="F12" s="6">
-        <v>-38757.717752456701</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="B13" s="6">
-        <v>616521.83971404994</v>
+        <v>-245350.52804946899</v>
       </c>
       <c r="C13" s="6">
-        <v>318424.66045618098</v>
+        <v>-149079.07512188001</v>
       </c>
       <c r="D13" s="6">
-        <v>272480.86318969697</v>
+        <v>-147393.917632103</v>
       </c>
       <c r="E13" s="6">
-        <v>138087.04233169599</v>
+        <v>-88860.592889785796</v>
       </c>
       <c r="F13" s="6">
-        <v>-40390.767657756798</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+        <v>-86007.295012474104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="6">
+        <v>-6740.3991222381601</v>
+      </c>
+      <c r="C14" s="6">
+        <v>22785.5114817619</v>
+      </c>
+      <c r="D14" s="6">
+        <v>-2038.8092756271401</v>
+      </c>
+      <c r="E14" s="6">
+        <v>-527.049779891968</v>
+      </c>
+      <c r="F14" s="6">
+        <v>-14370.839166641201</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" s="6">
-        <v>-245350.52804946899</v>
+        <v>6291.0391807556198</v>
       </c>
       <c r="C15" s="6">
-        <v>-149079.07512188001</v>
+        <v>5725.0028848648099</v>
       </c>
       <c r="D15" s="6">
-        <v>-147393.917632103</v>
+        <v>17269.913864135699</v>
       </c>
       <c r="E15" s="6">
-        <v>-88860.592889785796</v>
+        <v>3689.3484592437699</v>
       </c>
       <c r="F15" s="6">
-        <v>-86007.295012474104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+        <v>33205.348074436202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="6">
+        <v>-245799.887990952</v>
+      </c>
+      <c r="C16" s="6">
+        <v>-120568.560755253</v>
+      </c>
+      <c r="D16" s="6">
+        <v>-132162.81304359401</v>
+      </c>
+      <c r="E16" s="6">
+        <v>-85698.294210434004</v>
+      </c>
+      <c r="F16" s="6">
+        <v>-67172.786104679093</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="6">
-        <v>-6740.3991222381601</v>
-      </c>
-      <c r="C16" s="6">
-        <v>22785.5114817619</v>
-      </c>
-      <c r="D16" s="6">
-        <v>-2038.8092756271401</v>
-      </c>
-      <c r="E16" s="6">
-        <v>-527.049779891968</v>
-      </c>
-      <c r="F16" s="6">
-        <v>-14370.839166641201</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="6">
-        <v>6291.0391807556198</v>
-      </c>
-      <c r="C17" s="6">
-        <v>5725.0028848648099</v>
-      </c>
-      <c r="D17" s="6">
-        <v>17269.913864135699</v>
-      </c>
-      <c r="E17" s="6">
-        <v>3689.3484592437699</v>
-      </c>
-      <c r="F17" s="6">
-        <v>33205.348074436202</v>
-      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" s="6">
-        <v>-245799.887990952</v>
+        <v>-11683.358478546101</v>
       </c>
       <c r="C18" s="6">
-        <v>-120568.560755253</v>
+        <v>-19007.0095777512</v>
       </c>
       <c r="D18" s="6">
-        <v>-132162.81304359401</v>
+        <v>-14511.5248441696</v>
       </c>
       <c r="E18" s="6">
-        <v>-85698.294210434004</v>
+        <v>-45747.920894622803</v>
       </c>
       <c r="F18" s="6">
-        <v>-67172.786104679093</v>
+        <v>77297.695517540007</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="A19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6">
+        <v>-7976.1389613151596</v>
+      </c>
+      <c r="C19" s="6">
+        <v>164193.08273792299</v>
+      </c>
+      <c r="D19" s="6">
+        <v>18229.353523254402</v>
+      </c>
+      <c r="E19" s="6">
+        <v>9592.3059940338098</v>
+      </c>
+      <c r="F19" s="6">
+        <v>8056.3795328140304</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6">
+        <v>-79649.0496277809</v>
+      </c>
+      <c r="C20" s="6">
+        <v>-277662.63991594297</v>
+      </c>
+      <c r="D20" s="6">
+        <v>-29502.7695178986</v>
+      </c>
+      <c r="E20" s="6">
+        <v>-28249.868202209502</v>
+      </c>
+      <c r="F20" s="6">
+        <v>-53890.646874904603</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="6">
-        <v>-11683.358478546101</v>
-      </c>
-      <c r="C20" s="6">
-        <v>-19007.0095777512</v>
-      </c>
-      <c r="D20" s="6">
-        <v>-14511.5248441696</v>
-      </c>
-      <c r="E20" s="6">
-        <v>-45747.920894622803</v>
-      </c>
-      <c r="F20" s="6">
-        <v>77297.695517540007</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="B21" s="6">
+        <v>-207154.93302345299</v>
+      </c>
+      <c r="C21" s="6">
+        <v>-14427.007269859299</v>
+      </c>
+      <c r="D21" s="6">
+        <v>-2278.6691904068002</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="6">
-        <v>-7976.1389613151596</v>
-      </c>
-      <c r="C21" s="6">
-        <v>164193.08273792299</v>
-      </c>
-      <c r="D21" s="6">
-        <v>18229.353523254402</v>
-      </c>
-      <c r="E21" s="6">
-        <v>9592.3059940338098</v>
-      </c>
-      <c r="F21" s="6">
-        <v>8056.3795328140304</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="B22" s="6">
+        <v>-306463.48009109503</v>
+      </c>
+      <c r="C22" s="6">
+        <v>-146903.57402563101</v>
+      </c>
+      <c r="D22" s="6">
+        <v>-28063.610029220599</v>
+      </c>
+      <c r="E22" s="6">
+        <v>-64405.483102798498</v>
+      </c>
+      <c r="F22" s="6">
+        <v>31463.4281754494</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="6">
-        <v>-79649.0496277809</v>
-      </c>
-      <c r="C22" s="6">
-        <v>-277662.63991594297</v>
-      </c>
-      <c r="D22" s="6">
-        <v>-29502.7695178986</v>
-      </c>
-      <c r="E22" s="6">
-        <v>-28249.868202209502</v>
-      </c>
-      <c r="F22" s="6">
-        <v>-53890.646874904603</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="B24" s="6">
+        <v>-3145.5195903778099</v>
+      </c>
+      <c r="C24" s="6">
+        <v>4809.0024232864398</v>
+      </c>
+      <c r="D24" s="6">
+        <v>-6356.28774166107</v>
+      </c>
+      <c r="E24" s="6">
+        <v>-737.869691848755</v>
+      </c>
+      <c r="F24" s="6">
+        <v>7838.6395454406702</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="6">
-        <v>-207154.93302345299</v>
-      </c>
-      <c r="C23" s="6">
-        <v>-14427.007269859299</v>
-      </c>
-      <c r="D23" s="6">
-        <v>-2278.6691904068002</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="51" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="6">
-        <v>-306463.48009109503</v>
-      </c>
-      <c r="C24" s="6">
-        <v>-146903.57402563101</v>
-      </c>
-      <c r="D24" s="6">
-        <v>-28063.610029220599</v>
-      </c>
-      <c r="E24" s="6">
-        <v>-64405.483102798498</v>
-      </c>
-      <c r="F24" s="6">
-        <v>31463.4281754494</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="B25" s="6">
+        <v>61112.952041625998</v>
+      </c>
+      <c r="C25" s="6">
+        <v>55761.5280985832</v>
+      </c>
+      <c r="D25" s="6">
+        <v>105898.15237522101</v>
+      </c>
+      <c r="E25" s="6">
+        <v>-12754.6046733856</v>
+      </c>
+      <c r="F25" s="6">
+        <v>-68261.486041545897</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="6">
+        <v>520920.51216363901</v>
+      </c>
+      <c r="C26" s="6">
+        <v>475175.23944377899</v>
+      </c>
+      <c r="D26" s="6">
+        <v>391811.17079258</v>
+      </c>
+      <c r="E26" s="6">
+        <v>357128.93085479701</v>
+      </c>
+      <c r="F26" s="6">
+        <v>437113.02465200401</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="6">
-        <v>-3145.5195903778099</v>
-      </c>
-      <c r="C26" s="6">
-        <v>4809.0024232864398</v>
-      </c>
-      <c r="D26" s="6">
-        <v>-6356.28774166107</v>
-      </c>
-      <c r="E26" s="6">
-        <v>-737.869691848755</v>
-      </c>
-      <c r="F26" s="6">
-        <v>7838.6395454406702</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="B27" s="6">
-        <v>61112.952041625998</v>
+        <v>582033.46420526505</v>
       </c>
       <c r="C27" s="6">
-        <v>55761.5280985832</v>
+        <v>530936.76754236198</v>
       </c>
       <c r="D27" s="6">
-        <v>105898.15237522101</v>
+        <v>497709.32316780102</v>
       </c>
       <c r="E27" s="6">
-        <v>-12754.6046733856</v>
+        <v>344374.32618141198</v>
       </c>
       <c r="F27" s="6">
-        <v>-68261.486041545897</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="6">
-        <v>520920.51216363901</v>
-      </c>
-      <c r="C28" s="6">
-        <v>475175.23944377899</v>
-      </c>
-      <c r="D28" s="6">
-        <v>391811.17079258</v>
-      </c>
-      <c r="E28" s="6">
-        <v>357128.93085479701</v>
-      </c>
-      <c r="F28" s="6">
-        <v>437113.02465200401</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="6">
-        <v>582033.46420526505</v>
-      </c>
-      <c r="C29" s="6">
-        <v>530936.76754236198</v>
-      </c>
-      <c r="D29" s="6">
-        <v>497709.32316780102</v>
-      </c>
-      <c r="E29" s="6">
-        <v>344374.32618141198</v>
-      </c>
-      <c r="F29" s="6">
         <v>368851.53861045802</v>
       </c>
     </row>

</xml_diff>